<commit_message>
bletest-2: update xls bom
This file is not actually useful, as the html bom from the KiCad plugin
is much more useful.
</commit_message>
<xml_diff>
--- a/bletest-2/jolt-pcb-layout.xlsx
+++ b/bletest-2/jolt-pcb-layout.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidb/Documents/Keyboards/bletest-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A206C38-89DB-9D42-8DD2-4B398BC44345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2BEFE6-A474-284D-A1A4-043ECB16FBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{C908F1CD-26ED-6D4E-A411-B03D6EF96C7C}"/>
+    <workbookView xWindow="2020" yWindow="4940" windowWidth="31040" windowHeight="17700" xr2:uid="{C908F1CD-26ED-6D4E-A411-B03D6EF96C7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Jolt PCB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -402,6 +402,9 @@
               <c:separator>, </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C896-C740-B2D0-7569417F2E89}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -421,6 +424,9 @@
               <c:separator>, </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C896-C740-B2D0-7569417F2E89}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -440,6 +446,9 @@
               <c:separator>, </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-C896-C740-B2D0-7569417F2E89}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -481,6 +490,9 @@
               <c:separator>, </c:separator>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-C896-C740-B2D0-7569417F2E89}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1402,16 +1414,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>96006</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>408623</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>96227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122464</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>435081</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>21167</xdr:rowOff>
+      <xdr:rowOff>60244</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1756,15 +1768,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620A8F2B-91CD-4844-BE60-D4E6E99F7ADF}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-85</v>
       </c>
@@ -1785,8 +1797,16 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2">
+        <f>100-A2</f>
+        <v>185</v>
+      </c>
+      <c r="E2">
+        <f>100-B2</f>
+        <v>103</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-46</v>
       </c>
@@ -1796,8 +1816,16 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D16" si="0">100-A3</f>
+        <v>146</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E16" si="1">100-B3</f>
+        <v>103</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-46</v>
       </c>
@@ -1807,8 +1835,16 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-8</v>
       </c>
@@ -1818,8 +1854,16 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1829,8 +1873,16 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>64</v>
       </c>
@@ -1840,8 +1892,16 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>64</v>
       </c>
@@ -1851,8 +1911,16 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -1862,8 +1930,16 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1873,8 +1949,16 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-8</v>
       </c>
@@ -1884,8 +1968,16 @@
       <c r="C11" t="s">
         <v>11</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-8</v>
       </c>
@@ -1895,8 +1987,16 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-7</v>
       </c>
@@ -1906,8 +2006,16 @@
       <c r="C13" t="s">
         <v>13</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-61</v>
       </c>
@@ -1917,8 +2025,16 @@
       <c r="C14" t="s">
         <v>14</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-85</v>
       </c>
@@ -1928,8 +2044,16 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-85</v>
       </c>
@@ -1938,6 +2062,14 @@
       </c>
       <c r="C16" t="s">
         <v>16</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>185</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>